<commit_message>
Change files test02, test03
</commit_message>
<xml_diff>
--- a/test02.xlsx
+++ b/test02.xlsx
@@ -4859,105 +4859,165 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+A1</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f>G2+G1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+A2</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f>G3+G2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A16" si="0">A4+A3</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f t="shared" ref="G5:G16" si="1">G4+G3</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>144</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>233</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>377</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>610</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>610</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>987</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>987</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
+        <v>1597</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
         <v>1597</v>
       </c>
     </row>

</xml_diff>